<commit_message>
fin de projet, dernier commit
</commit_message>
<xml_diff>
--- a/plan de test.xlsx
+++ b/plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom85\Documents\Formation OPCL\Projet 5\Production\TomPascreau_5_21042021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73305402-6D5F-48E9-B44B-8C4AD5938BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C0D67-D62D-4847-95A4-FFA9D4B92F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -43,71 +43,116 @@
     <t>script.js</t>
   </si>
   <si>
-    <t>rentrer pour chaque champ : chaine vide, chaine sans lettres (uniquement caractères spéciaux ou chiffres), chaine avec caractères spéciaux et lettres. pour validityNames, validityMail et testEmail tester avec des chiffres. Pour validityMail et testEmail tester sans arobase.</t>
+    <t>4 à 25</t>
   </si>
   <si>
-    <t>96 à 124</t>
+    <t>chargeProduit</t>
   </si>
   <si>
-    <t>la valeur retournée pourrait être erronée (0 au lieu de 1; et 1 au lieu de 0). Le message d'erreur correspond au champ testé (exemple : ville incorrecte pour le champ ville)</t>
+    <t xml:space="preserve">La fonction doit créer une card par article envoyé par l'API avec le nom, l'image et le prix pour tous les produits </t>
   </si>
   <si>
-    <t>126 à 132</t>
+    <t xml:space="preserve">La fonction pourrait oublier un ou des articles ou remplir un champ avec une mauvaise information. </t>
   </si>
   <si>
-    <t>réaliser un console.log de productId et vérifier que la quantité de valeurs contenues dans le tableau correspond au nombre d'articles dans le panier</t>
+    <t>31 à 46</t>
   </si>
   <si>
-    <t>la fonction pourrait ajouter un nombre trop important d'Id ou ne pas les ajouter du tout</t>
+    <t>chargeDetailsProduits</t>
   </si>
   <si>
-    <t>la fonction doit retourner 1 si les valeurs entrées dans le formulaire sont correctes et si il y a des articles dans le panier</t>
+    <t>La fonction doit charger les infromations du produits ayant pour Id celui passé en paramètre dans l'URL</t>
   </si>
   <si>
-    <t>la fonction pourrait valider l'envoi du formulaire avec des mauvaises données ou envoyer une commande avec un panier vide</t>
+    <t>Faire un console log de "data" et vérifier que l'id de l'URL correspond à l'Id de data conformément au clic sur le produit choisi</t>
   </si>
   <si>
-    <t xml:space="preserve">entrer des valeurs limites pour le formulaire (cf.validCommand partie 1) et essayer de soumettre le formulaire avec un panier vide </t>
+    <t>La fonction pourrait charger un mauvais produit ou aucun produit</t>
   </si>
   <si>
-    <t>86 à 162</t>
+    <t>52 à 61</t>
   </si>
   <si>
-    <t>134 à 137</t>
+    <t>addToCart</t>
   </si>
   <si>
-    <t>validCommand partie 3</t>
+    <t>La focntion doit ajouter l'Id de l'article à ajouter au panier dans localStorage uniquement si il n'y est pas déjà.</t>
   </si>
   <si>
-    <t>validCommand partie 2</t>
+    <t>Faire un console log de localStorage après le clic et vérifier la présence de l'Id du produit</t>
   </si>
   <si>
-    <t>validCommand partie 1</t>
+    <t>La fonction pourrait ne pas ajouter l'Id ou l'ajouter plusieurs fois.</t>
   </si>
   <si>
-    <t>vider le panier et tenter de soumettre le formulaire</t>
+    <t>68 à 93</t>
   </si>
   <si>
-    <t>la fonction pourrait retourner true au lieu de false et false au lieu de true</t>
+    <t>chargeCartProducts</t>
   </si>
   <si>
-    <t>validCommand globale</t>
+    <t>La fonction récupère la data de l'API et les Id de localStorage. Pour chaque correspondance entre les Id de la data et de localStorage, une card est créée avec l'image, le nom, le prix, et l'Id du produit.</t>
   </si>
   <si>
-    <t>Cette partie de la fonction doit retourner false si il n'y a pas d'articles dans la panier</t>
+    <t>faire des console log de data et localStorage et vérifier les correspondances entre les deux et le nombre de cards créées</t>
   </si>
   <si>
-    <t>cette partie de la fonction doit ajouter les id contenues dans localStorage au tableau productId</t>
+    <t>La fonction pourrait créer un nombre de cards qui ne correpond pas aux nombres de correpondances d'id entre les deux sources de données (localStorage et data).</t>
   </si>
   <si>
-    <t>Cette partie de la fonction doit retourner false si la saisie ne correspond pas à l'epression régulière lui correspondant : validityNames pour le prénom, nom de famille, et ville; validityAddress pour l'adresse (ajout des chiffres); validityMail et testEmail pour le mail (ajout du point et de l'arobase et verification de la présence de l'arobase)</t>
+    <t>Faire un console log de "data" et comparer le nombre de produits dans la data et le nombre de cards affichées par la page web</t>
+  </si>
+  <si>
+    <t>99 à 102</t>
+  </si>
+  <si>
+    <t>removeItemCart</t>
+  </si>
+  <si>
+    <t>La focntion supprime un Id de localStorage et rafraichit la page</t>
+  </si>
+  <si>
+    <t>Faire un console log de localStorage, supprimer un produit du panier et vérifier la suppression de l'Id de l'article supprimé dans localStorage.</t>
+  </si>
+  <si>
+    <t>La fonction pourrait ne pas supprimer l'Id ou ne pas rafraichir la page.</t>
+  </si>
+  <si>
+    <t>110 à 186</t>
+  </si>
+  <si>
+    <t>validCommand</t>
+  </si>
+  <si>
+    <t>La fonction pourrait laisser le formulaire se soumettre avec des données invalides ou avec un panier vide ce qui pourait créer une erreur.</t>
+  </si>
+  <si>
+    <t>La fonction vérifie la validité de chaque champ du formulaire, stocke les Id contenues dans localStorage dans un tableau, vérifie que le panier ne soit pas vide, fait une requete fetch avec POST, récupère l'Id de commande retourné par l'API, redirige vers la page de confirmation de commande et vide localStorage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rentrer des données invalides dans le formulaire (chaine vide, caractères spéciaux…), ou essayer de valider la commande avec un panier vide. Faire un console log de localStorage pour vérifier qu'il soit vide </t>
+  </si>
+  <si>
+    <t>191 à 194</t>
+  </si>
+  <si>
+    <t>checkCommand</t>
+  </si>
+  <si>
+    <t>La fonction récupère l'Id stocké dans l'URL et le positionne dans la page de confirmation de commande.</t>
+  </si>
+  <si>
+    <t>vérifier que l'Id dans l'URL correspond à l'url affiché dans la page de confirmation.</t>
+  </si>
+  <si>
+    <t>L'Id affiché pourrait ne pas correspondre à l'Id stocké dans l'URL.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,6 +170,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -396,8 +445,8 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -460,19 +509,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -480,19 +529,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -500,19 +549,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -520,35 +569,80 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="6"/>
@@ -5496,6 +5590,7 @@
       <c r="F998" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>